<commit_message>
LDA revised and finished optimization
</commit_message>
<xml_diff>
--- a/Project_python/out/LDA/optimization.xlsx
+++ b/Project_python/out/LDA/optimization.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -506,147 +506,11 @@
         <v>38.41463414634146</v>
       </c>
       <c r="I2" t="n">
-        <v>-7.277963896428299</v>
+        <v>-7.277964451628145</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
           <t>x1:1.15|x2:0.68|x3:1.00|x4:0.75|x5:1.00|x6:1.00|x7:1.22|x8:1.48|x9:0.84|x10:1.00|x11:1.11|x12:1.29|x13:1.30|x14:1.00|x15:1.00|x16:1.19|x17:0.00</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="n">
-        <v>17</v>
-      </c>
-      <c r="C3" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D3" t="n">
-        <v>100</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="F3" t="b">
-        <v>1</v>
-      </c>
-      <c r="G3" t="n">
-        <v>34.14634146341464</v>
-      </c>
-      <c r="H3" t="n">
-        <v>36.58536585365854</v>
-      </c>
-      <c r="I3" t="n">
-        <v>-7.317862736538368</v>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>x1:0.71|x2:1.23|x3:1.00|x4:0.57|x5:0.84|x6:1.00|x7:1.10|x8:1.16|x9:1.30|x10:1.41|x11:0.51|x12:1.06|x13:1.34|x14:1.48|x15:1.00|x16:1.27|x17:0.00</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
-        <v>17</v>
-      </c>
-      <c r="C4" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D4" t="n">
-        <v>1000</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="F4" t="b">
-        <v>1</v>
-      </c>
-      <c r="G4" t="n">
-        <v>31.09756097560976</v>
-      </c>
-      <c r="H4" t="n">
-        <v>33.53658536585366</v>
-      </c>
-      <c r="I4" t="n">
-        <v>-7.325163373011051</v>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>x1:0.72|x2:1.35|x3:1.00|x4:0.46|x5:0.54|x6:1.00|x7:1.10|x8:1.00|x9:1.30|x10:1.44|x11:0.51|x12:0.82|x13:1.75|x14:1.68|x15:1.00|x16:1.34|x17:0.00</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="n">
-        <v>17</v>
-      </c>
-      <c r="C5" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D5" t="n">
-        <v>400</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="F5" t="b">
-        <v>1</v>
-      </c>
-      <c r="G5" t="n">
-        <v>30.48780487804878</v>
-      </c>
-      <c r="H5" t="n">
-        <v>34.14634146341464</v>
-      </c>
-      <c r="I5" t="n">
-        <v>-7.323880143913545</v>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>x1:0.72|x2:1.50|x3:1.00|x4:0.45|x5:0.55|x6:1.00|x7:0.83|x8:1.00|x9:1.30|x10:1.50|x11:0.64|x12:0.87|x13:1.66|x14:1.67|x15:1.00|x16:1.31|x17:0.00</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="n">
-        <v>17</v>
-      </c>
-      <c r="C6" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D6" t="n">
-        <v>600</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="F6" t="b">
-        <v>1</v>
-      </c>
-      <c r="G6" t="n">
-        <v>31.70731707317073</v>
-      </c>
-      <c r="H6" t="n">
-        <v>34.14634146341464</v>
-      </c>
-      <c r="I6" t="n">
-        <v>-7.324917490819145</v>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>x1:0.72|x2:1.36|x3:1.00|x4:0.45|x5:0.55|x6:1.00|x7:1.08|x8:1.00|x9:1.31|x10:1.47|x11:0.52|x12:0.84|x13:1.73|x14:1.65|x15:1.00|x16:1.32|x17:0.00</t>
         </is>
       </c>
     </row>

</xml_diff>